<commit_message>
Not gluten free - wheat filering.
</commit_message>
<xml_diff>
--- a/vocab.xlsx
+++ b/vocab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="12180" windowWidth="37520" windowHeight="16500"/>
+    <workbookView xWindow="2200" yWindow="12680" windowWidth="37120" windowHeight="13820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="220">
   <si>
     <t>Preferred</t>
   </si>
@@ -159,12 +159,6 @@
     <t>gamma-HCH</t>
   </si>
   <si>
-    <t>BHC - gamma (Lindane)</t>
-  </si>
-  <si>
-    <t>BHC-gamma (Lindane)</t>
-  </si>
-  <si>
     <t>HCH-gamma (Lindane)</t>
   </si>
   <si>
@@ -258,15 +252,6 @@
     <t>HCH-Total</t>
   </si>
   <si>
-    <t>BHC (alpha)</t>
-  </si>
-  <si>
-    <t>BHC (beta)</t>
-  </si>
-  <si>
-    <t>BHC (delta)</t>
-  </si>
-  <si>
     <t>BHC-alpha</t>
   </si>
   <si>
@@ -342,15 +327,9 @@
     <t>Clothiandin</t>
   </si>
   <si>
-    <t>Cyfluthrin Î²</t>
-  </si>
-  <si>
     <t>Cyhalothrin-lambda</t>
   </si>
   <si>
-    <t>Cyhalothrin Î»</t>
-  </si>
-  <si>
     <t>Cypermethrin Î¬</t>
   </si>
   <si>
@@ -369,21 +348,12 @@
     <t>Deltamethrin</t>
   </si>
   <si>
-    <t>Deltamethrin (cis &amp; trans)</t>
-  </si>
-  <si>
     <t>Difenoconazole</t>
   </si>
   <si>
-    <t>Difenoconazole (cis &amp; trans)</t>
-  </si>
-  <si>
     <t>Dimethomorph</t>
   </si>
   <si>
-    <t>Dimethomorph (-E&amp;Z)</t>
-  </si>
-  <si>
     <t>Disulfoton</t>
   </si>
   <si>
@@ -414,21 +384,12 @@
     <t>Endosulfan-alpha</t>
   </si>
   <si>
-    <t>Endosulfan (beta)</t>
-  </si>
-  <si>
     <t>Endosulfan sulphate</t>
   </si>
   <si>
     <t>Endosulfan sulfate</t>
   </si>
   <si>
-    <t>Endosulfan Î¬</t>
-  </si>
-  <si>
-    <t>Endosulfan (alpha)</t>
-  </si>
-  <si>
     <t>Endosulfan - Sulphate</t>
   </si>
   <si>
@@ -600,15 +561,9 @@
     <t>Permethrin</t>
   </si>
   <si>
-    <t>Permethrin (cis &amp; trans)</t>
-  </si>
-  <si>
     <t>Phenothrin</t>
   </si>
   <si>
-    <t>Phenothrin (cis &amp; trans)</t>
-  </si>
-  <si>
     <t>Piperonyl butoxide</t>
   </si>
   <si>
@@ -633,9 +588,6 @@
     <t xml:space="preserve">Pyrethrins </t>
   </si>
   <si>
-    <t>Pyrethrins (sum of positives)</t>
-  </si>
-  <si>
     <t>Pyriproxyfen</t>
   </si>
   <si>
@@ -694,6 +646,45 @@
   </si>
   <si>
     <t>Zeta cypermethrin</t>
+  </si>
+  <si>
+    <t>BHC \(alpha\)</t>
+  </si>
+  <si>
+    <t>BHC \(delta\)</t>
+  </si>
+  <si>
+    <t>BHC - gamma \(Lindane\)</t>
+  </si>
+  <si>
+    <t>BHC \(beta\)</t>
+  </si>
+  <si>
+    <t>BHC-gamma \(Lindane\)</t>
+  </si>
+  <si>
+    <t>Endosulfan \(alpha\)</t>
+  </si>
+  <si>
+    <t>Endosulfan \(beta\)</t>
+  </si>
+  <si>
+    <t>Difenoconazole \(cis &amp; trans\)</t>
+  </si>
+  <si>
+    <t>Dimethomorph \(-E&amp;Z\)</t>
+  </si>
+  <si>
+    <t>Deltamethrin \(cis &amp; trans\)</t>
+  </si>
+  <si>
+    <t>Permethrin \(cis &amp; trans\)</t>
+  </si>
+  <si>
+    <t>Phenothrin \(cis &amp; trans\)</t>
+  </si>
+  <si>
+    <t>Pyrethrins \(sum of positives\)</t>
   </si>
 </sst>
 </file>
@@ -742,8 +733,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -758,17 +751,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1047,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1076,10 +1071,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1109,570 +1104,588 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>157</v>
+      </c>
+      <c r="C18" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
-      </c>
-      <c r="C20" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>204</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>220</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>222</v>
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" t="s">
-        <v>42</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>183</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>123</v>
+        <v>120</v>
+      </c>
+      <c r="C37" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B40" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>124</v>
+      </c>
+      <c r="D40" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
-      </c>
-      <c r="D42" t="s">
-        <v>138</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B49" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B54" t="s">
-        <v>158</v>
+        <v>191</v>
+      </c>
+      <c r="C54" t="s">
+        <v>193</v>
+      </c>
+      <c r="D54" t="s">
+        <v>194</v>
+      </c>
+      <c r="E54" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>159</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>208</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
         <v>207</v>
       </c>
-      <c r="C56" t="s">
-        <v>209</v>
-      </c>
       <c r="D56" t="s">
-        <v>210</v>
-      </c>
-      <c r="E56" t="s">
-        <v>211</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="C57" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" t="s">
+        <v>69</v>
+      </c>
+      <c r="E57" t="s">
+        <v>210</v>
+      </c>
+      <c r="F57" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
+        <v>208</v>
+      </c>
+      <c r="D58" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" t="s">
         <v>77</v>
       </c>
-      <c r="D58" t="s">
-        <v>80</v>
+      <c r="F58" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>211</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>209</v>
       </c>
       <c r="D59" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
-      </c>
-      <c r="F59" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1682,228 +1695,191 @@
       <c r="B60" t="s">
         <v>73</v>
       </c>
-      <c r="C60" t="s">
-        <v>79</v>
-      </c>
-      <c r="D60" t="s">
-        <v>112</v>
-      </c>
-      <c r="E60" t="s">
-        <v>82</v>
-      </c>
-      <c r="F60" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" t="s">
-        <v>44</v>
-      </c>
-      <c r="D61" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
         <v>163</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B67" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
         <v>165</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B68" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>167</v>
-      </c>
-      <c r="B66" t="s">
-        <v>168</v>
-      </c>
-      <c r="C66" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" t="s">
         <v>172</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C69" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
         <v>174</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
+      <c r="C70" t="s">
         <v>176</v>
       </c>
-      <c r="B69" t="s">
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
+      <c r="B71" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
         <v>178</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
+      <c r="B73" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>181</v>
+      </c>
+      <c r="B74" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>183</v>
+      </c>
+      <c r="B75" t="s">
         <v>184</v>
       </c>
-      <c r="B71" t="s">
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
         <v>185</v>
       </c>
-      <c r="C71" t="s">
+      <c r="B76" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
+      <c r="C76" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
         <v>187</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B77" t="s">
         <v>188</v>
       </c>
-      <c r="C72" t="s">
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
+      <c r="B78" t="s">
         <v>190</v>
       </c>
-      <c r="B73" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>192</v>
-      </c>
-      <c r="B74" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>194</v>
-      </c>
-      <c r="B75" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
         <v>196</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B79" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
+      <c r="C79" t="s">
         <v>198</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D79" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
         <v>200</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B80" t="s">
         <v>201</v>
       </c>
-      <c r="C78" t="s">
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+      <c r="B81" t="s">
         <v>203</v>
-      </c>
-      <c r="B79" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>205</v>
-      </c>
-      <c r="B80" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" t="s">
-        <v>212</v>
-      </c>
-      <c r="B81" t="s">
-        <v>213</v>
-      </c>
-      <c r="C81" t="s">
-        <v>214</v>
-      </c>
-      <c r="D81" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" t="s">
-        <v>216</v>
-      </c>
-      <c r="B82" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" t="s">
-        <v>218</v>
-      </c>
-      <c r="B83" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fiddling with asian set
</commit_message>
<xml_diff>
--- a/vocab.xlsx
+++ b/vocab.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub Projects\Pesticide_Compilation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="12675" windowWidth="37125" windowHeight="13815"/>
+    <workbookView xWindow="2900" yWindow="1180" windowWidth="40180" windowHeight="26560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,20 +12,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="225">
   <si>
     <t>Preferred</t>
   </si>
@@ -699,6 +694,12 @@
   </si>
   <si>
     <t>Demeton-S-Methyl</t>
+  </si>
+  <si>
+    <t>Endosulphan sulphate</t>
+  </si>
+  <si>
+    <t>Endosulphan-Total</t>
   </si>
 </sst>
 </file>
@@ -747,8 +748,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -765,19 +774,27 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1048,7 +1065,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1056,19 +1073,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="7" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="7" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1108,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1108,7 +1125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1116,7 +1133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1124,7 +1141,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1132,7 +1149,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1140,7 +1157,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -1148,7 +1165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -1156,7 +1173,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -1167,7 +1184,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -1175,7 +1192,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1183,7 +1200,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -1191,7 +1208,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -1199,7 +1216,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -1207,7 +1224,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -1218,7 +1235,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -1226,7 +1243,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1234,7 +1251,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -1245,7 +1262,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1256,7 +1273,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1264,7 +1281,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>205</v>
       </c>
@@ -1275,7 +1292,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -1283,7 +1300,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1300,7 +1317,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1317,7 +1334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1334,7 +1351,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1351,7 +1368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1368,7 +1385,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1385,7 +1402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -1393,7 +1410,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -1401,7 +1418,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>170</v>
       </c>
@@ -1409,7 +1426,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>107</v>
       </c>
@@ -1417,7 +1434,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1425,7 +1442,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -1436,7 +1453,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>112</v>
       </c>
@@ -1444,7 +1461,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -1452,9 +1469,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>223</v>
       </c>
       <c r="B37" t="s">
         <v>120</v>
@@ -1462,448 +1479,450 @@
       <c r="C37" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
+        <v>224</v>
+      </c>
+      <c r="B38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" t="s">
         <v>118</v>
       </c>
-      <c r="B38" t="s">
+      <c r="E39" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s">
         <v>116</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E40" t="s">
         <v>117</v>
       </c>
-      <c r="C39" t="s">
+      <c r="F40" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>122</v>
-      </c>
-      <c r="B40" t="s">
-        <v>123</v>
-      </c>
-      <c r="C40" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B46" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="C52" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52" t="s">
+        <v>194</v>
+      </c>
+      <c r="E52" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>191</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="D54" t="s">
-        <v>194</v>
-      </c>
-      <c r="E54" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" t="s">
+        <v>210</v>
+      </c>
+      <c r="F55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D56" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>211</v>
       </c>
       <c r="C57" t="s">
-        <v>68</v>
+        <v>209</v>
       </c>
       <c r="D57" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="E57" t="s">
-        <v>210</v>
-      </c>
-      <c r="F57" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
-      </c>
-      <c r="C58" t="s">
-        <v>208</v>
-      </c>
-      <c r="D58" t="s">
-        <v>105</v>
-      </c>
-      <c r="E58" t="s">
-        <v>77</v>
-      </c>
-      <c r="F58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="B59" t="s">
-        <v>211</v>
-      </c>
-      <c r="C59" t="s">
-        <v>209</v>
-      </c>
-      <c r="D59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E59" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="C62" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B64" t="s">
-        <v>155</v>
-      </c>
-      <c r="C64" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B65" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B67" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="C67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="C68" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B69" t="s">
-        <v>172</v>
-      </c>
-      <c r="C69" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B70" t="s">
-        <v>175</v>
-      </c>
-      <c r="C70" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B72" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B73" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B74" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="C74" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B75" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B76" t="s">
-        <v>186</v>
-      </c>
-      <c r="C76" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B77" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="C77" t="s">
+        <v>198</v>
+      </c>
+      <c r="D77" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="B78" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B79" t="s">
-        <v>197</v>
-      </c>
-      <c r="C79" t="s">
-        <v>198</v>
-      </c>
-      <c r="D79" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="B80" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>202</v>
-      </c>
-      <c r="B81" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>220</v>
-      </c>
-      <c r="B82" t="s">
         <v>221</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C80" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Getting the wretched thing to work, at last!
</commit_message>
<xml_diff>
--- a/vocab.xlsx
+++ b/vocab.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="1180" windowWidth="40180" windowHeight="26560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40520" windowHeight="25280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="231">
   <si>
     <t>Preferred</t>
   </si>
@@ -700,6 +700,24 @@
   </si>
   <si>
     <t>Endosulphan-Total</t>
+  </si>
+  <si>
+    <t>Endosulfan alpha</t>
+  </si>
+  <si>
+    <t>Endosulphan</t>
+  </si>
+  <si>
+    <t>Endosulfan</t>
+  </si>
+  <si>
+    <t>Demeton-s-methylsulfoxide</t>
+  </si>
+  <si>
+    <t>Demeton-S-methylsulfoxide</t>
+  </si>
+  <si>
+    <t>Filter</t>
   </si>
 </sst>
 </file>
@@ -748,7 +766,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -770,11 +788,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -785,6 +812,9 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -795,6 +825,9 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1073,863 +1106,1129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="7" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="8" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>58</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>81</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>82</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>86</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>87</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>90</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>96</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>91</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>93</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>94</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>98</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>100</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>157</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>48</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>205</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>204</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>102</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>29</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>35</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>38</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>14</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>18</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>37</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>11</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>25</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>13</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>36</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>39</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>15</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>17</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>19</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>106</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C30" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" t="s">
+        <v>221</v>
+      </c>
+      <c r="D31" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>168</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C32" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>170</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C33" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>107</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C34" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
+    <row r="35" spans="1:7">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>108</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C35" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
+    <row r="36" spans="1:7">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>109</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C36" t="s">
         <v>110</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D36" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
+    <row r="37" spans="1:7">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>112</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C37" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
+    <row r="38" spans="1:7">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>114</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C38" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>223</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C40" t="s">
         <v>120</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D40" t="s">
         <v>121</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E40" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
+    <row r="41" spans="1:7">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
         <v>224</v>
       </c>
-      <c r="B38" t="s">
-        <v>123</v>
-      </c>
-      <c r="C38" t="s">
-        <v>124</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E41" t="s">
         <v>125</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F41" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
+    <row r="42" spans="1:7">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>51</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C42" t="s">
         <v>50</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D42" t="s">
         <v>52</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E42" t="s">
         <v>118</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F42" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
+      <c r="G42" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>226</v>
+      </c>
+      <c r="C43" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>192</v>
+      </c>
+      <c r="C55" t="s">
+        <v>191</v>
+      </c>
+      <c r="D55" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" t="s">
+        <v>194</v>
+      </c>
+      <c r="F55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" t="s">
+        <v>207</v>
+      </c>
+      <c r="E57" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" t="s">
+        <v>69</v>
+      </c>
+      <c r="F58" t="s">
+        <v>210</v>
+      </c>
+      <c r="G58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" t="s">
+        <v>208</v>
+      </c>
+      <c r="E59" t="s">
+        <v>105</v>
+      </c>
+      <c r="F59" t="s">
+        <v>77</v>
+      </c>
+      <c r="G59" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60" t="s">
+        <v>211</v>
+      </c>
+      <c r="D60" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>154</v>
+      </c>
+      <c r="C65" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>161</v>
+      </c>
+      <c r="C67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B40" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" t="s">
-        <v>117</v>
-      </c>
-      <c r="F40" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>126</v>
-      </c>
-      <c r="B41" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B44" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>136</v>
-      </c>
-      <c r="B46" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
-        <v>192</v>
-      </c>
-      <c r="B52" t="s">
-        <v>191</v>
-      </c>
-      <c r="C52" t="s">
-        <v>193</v>
-      </c>
-      <c r="D52" t="s">
-        <v>194</v>
-      </c>
-      <c r="E52" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="B68" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>171</v>
+      </c>
+      <c r="C70" t="s">
+        <v>172</v>
+      </c>
+      <c r="D70" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="C54" t="s">
-        <v>207</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="B71" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" t="s">
+        <v>175</v>
+      </c>
+      <c r="D71" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>181</v>
+      </c>
+      <c r="C75" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" t="s">
-        <v>69</v>
-      </c>
-      <c r="E55" t="s">
-        <v>210</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="B76" t="s">
+        <v>183</v>
+      </c>
+      <c r="C76" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
-        <v>72</v>
-      </c>
-      <c r="B56" t="s">
-        <v>71</v>
-      </c>
-      <c r="C56" t="s">
-        <v>208</v>
-      </c>
-      <c r="D56" t="s">
-        <v>105</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="B77" t="s">
+        <v>185</v>
+      </c>
+      <c r="C77" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="F56" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57" t="s">
-        <v>211</v>
-      </c>
-      <c r="C57" t="s">
-        <v>209</v>
-      </c>
-      <c r="D57" t="s">
-        <v>24</v>
-      </c>
-      <c r="E57" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>148</v>
-      </c>
-      <c r="B59" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>150</v>
-      </c>
-      <c r="B60" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>152</v>
-      </c>
-      <c r="B61" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B62" t="s">
-        <v>155</v>
-      </c>
-      <c r="C62" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>159</v>
-      </c>
-      <c r="B63" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>161</v>
-      </c>
-      <c r="B64" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>163</v>
-      </c>
-      <c r="B65" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>165</v>
-      </c>
-      <c r="B66" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
-        <v>171</v>
-      </c>
-      <c r="B67" t="s">
-        <v>172</v>
-      </c>
-      <c r="C67" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
-        <v>174</v>
-      </c>
-      <c r="B68" t="s">
-        <v>175</v>
-      </c>
-      <c r="C68" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>177</v>
-      </c>
-      <c r="B69" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
-        <v>178</v>
-      </c>
-      <c r="B70" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
-        <v>179</v>
-      </c>
-      <c r="B71" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" t="s">
-        <v>181</v>
-      </c>
-      <c r="B72" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" t="s">
-        <v>183</v>
-      </c>
-      <c r="B73" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
-        <v>185</v>
-      </c>
-      <c r="B74" t="s">
-        <v>186</v>
-      </c>
-      <c r="C74" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" t="s">
+      <c r="B78" t="s">
         <v>187</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C78" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
+    <row r="79" spans="1:5">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
         <v>189</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C79" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="s">
+    <row r="80" spans="1:5">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
         <v>196</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C80" t="s">
         <v>197</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D80" t="s">
         <v>198</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E80" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" t="s">
+    <row r="81" spans="1:3">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
         <v>200</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C81" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
         <v>202</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C82" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" t="s">
-        <v>220</v>
-      </c>
-      <c r="B80" t="s">
-        <v>221</v>
-      </c>
-      <c r="C80" t="s">
-        <v>222</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G1">
-    <sortState ref="A2:G86">
-      <sortCondition ref="A1:A86"/>
+  <autoFilter ref="A1:H1">
+    <sortState ref="A2:H82">
+      <sortCondition ref="A1:A82"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Annotated combined_pesticides, added to vocab
</commit_message>
<xml_diff>
--- a/vocab.xlsx
+++ b/vocab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1860" windowWidth="40900" windowHeight="23240"/>
+    <workbookView xWindow="12120" yWindow="1860" windowWidth="35140" windowHeight="23240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="286">
   <si>
     <t>Preferred</t>
   </si>
@@ -874,6 +874,15 @@
   </si>
   <si>
     <t>D-BHC</t>
+  </si>
+  <si>
+    <t>DDD-p,p</t>
+  </si>
+  <si>
+    <t>DDE-p,p</t>
+  </si>
+  <si>
+    <t>DDT-p,p</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1416,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:XFD88"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1636,7 +1645,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>80</v>
       </c>
@@ -1647,7 +1656,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>85</v>
       </c>
@@ -1664,7 +1673,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>90</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>95</v>
       </c>
@@ -1689,7 +1698,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>100</v>
       </c>
@@ -1703,7 +1712,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>105</v>
       </c>
@@ -1714,7 +1723,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>107</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>110</v>
       </c>
@@ -1754,7 +1763,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>115</v>
       </c>
@@ -1779,8 +1788,11 @@
       <c r="H25" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>120</v>
       </c>
@@ -1806,7 +1818,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>125</v>
       </c>
@@ -1831,8 +1843,11 @@
       <c r="H27" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>130</v>
       </c>
@@ -1858,7 +1873,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>135</v>
       </c>
@@ -1883,8 +1898,11 @@
       <c r="H29" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>140</v>
       </c>
@@ -1895,7 +1913,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>145</v>
       </c>
@@ -1909,7 +1927,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>150</v>
       </c>

</xml_diff>